<commit_message>
Excel menu added to Celery task
</commit_message>
<xml_diff>
--- a/app/admin/Menu.xlsx
+++ b/app/admin/Menu.xlsx
@@ -22,19 +22,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
-    <t xml:space="preserve">Закусон</t>
+    <t xml:space="preserve">Закуски</t>
   </si>
   <si>
     <t xml:space="preserve">описание меню закусок</t>
   </si>
   <si>
-    <t xml:space="preserve">Холодные куски-закуски</t>
+    <t xml:space="preserve">Холодные</t>
   </si>
   <si>
     <t xml:space="preserve">описание подменю закусок</t>
   </si>
   <si>
-    <t xml:space="preserve">Сельдь Бисмарк</t>
+    <t xml:space="preserve">Сельдь Бисмарк fish</t>
   </si>
   <si>
     <t xml:space="preserve">Традиционное немецкое блюдо из маринованной сельди</t>
@@ -52,7 +52,7 @@
     <t xml:space="preserve">Нарезка из креветок, кальмаров, раковых шеек, гребешков, лосося, скумбрии и красной икры</t>
   </si>
   <si>
-    <t xml:space="preserve">Рамен супчики</t>
+    <t xml:space="preserve">Рамен</t>
   </si>
   <si>
     <t xml:space="preserve">описание подменю супов</t>
@@ -226,7 +226,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -287,10 +287,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -310,16 +306,16 @@
   </sheetPr>
   <dimension ref="A1:F996"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="35.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="35.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="77.71"/>
   </cols>
   <sheetData>
@@ -609,19 +605,19 @@
       <c r="C21" s="13"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
+      <c r="F21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C22" s="13"/>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
+      <c r="F22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C23" s="13"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
+      <c r="F23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C24" s="12"/>
@@ -631,13 +627,13 @@
       <c r="C25" s="13"/>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
+      <c r="F25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C26" s="13"/>
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
+      <c r="F26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>